<commit_message>
update of input file
</commit_message>
<xml_diff>
--- a/input/COSPIN_input.xlsx
+++ b/input/COSPIN_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muji\source\1DSolver\1D Solver\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FKMV\Desktop\COSPIN\1D Solver\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5110E096-D37B-44A1-85FD-7C964A07968B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9927664-08F1-4102-9039-7414B575C6AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="668" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="1416" windowWidth="23256" windowHeight="12576" tabRatio="668" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOCATIONS" sheetId="1" r:id="rId1"/>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="354">
   <si>
     <t>SRD model</t>
   </si>
@@ -1198,39 +1198,6 @@
   </si>
   <si>
     <t>lateral_load_deflection_DNV_1</t>
-  </si>
-  <si>
-    <t>export_springs_Diam5</t>
-  </si>
-  <si>
-    <t>export_springs_Diam7</t>
-  </si>
-  <si>
-    <t>export_springs_Diam8</t>
-  </si>
-  <si>
-    <t>export_springs_Diam9</t>
-  </si>
-  <si>
-    <t>export_springs_Diam10</t>
-  </si>
-  <si>
-    <t>export_springs_Diam11</t>
-  </si>
-  <si>
-    <t>export_springs_Diam13</t>
-  </si>
-  <si>
-    <t>export_springs_Diam14</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>analysis 1</t>
   </si>
   <si>
     <t>lateral_load_rotation_pile_length_effect</t>
@@ -3616,6 +3583,15 @@
     </xf>
     <xf numFmtId="3" fontId="11" fillId="9" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="9" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="9" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="9" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="3" fontId="11" fillId="9" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3625,15 +3601,6 @@
     <xf numFmtId="3" fontId="11" fillId="9" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="9" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="9" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="9" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -9815,16 +9782,16 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="+hejb9GmU5MbBslfF0G+hOuLh3Tjbkw4IYn0RKdA3nzcGHlszpBvaRxpZw3IQ8CmMLm76eFnL3xmWI9NkFle9A==" saltValue="RZkuZJdGRHxlXAMqhau3aA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="10">
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="AJ1:AM1"/>
+    <mergeCell ref="AN1:AQ1"/>
+    <mergeCell ref="AR1:AU1"/>
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="P1:S1"/>
     <mergeCell ref="T1:W1"/>
     <mergeCell ref="X1:AA1"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="AJ1:AM1"/>
-    <mergeCell ref="AN1:AQ1"/>
-    <mergeCell ref="AR1:AU1"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12318,8 +12285,8 @@
   </sheetPr>
   <dimension ref="A1:BP2237"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12353,76 +12320,76 @@
       <c r="A1" s="313"/>
       <c r="B1" s="313"/>
       <c r="C1" s="160"/>
-      <c r="D1" s="371" t="s">
+      <c r="D1" s="368" t="s">
         <v>311</v>
       </c>
-      <c r="E1" s="372"/>
-      <c r="F1" s="372"/>
-      <c r="G1" s="372"/>
-      <c r="H1" s="373"/>
-      <c r="I1" s="371" t="s">
+      <c r="E1" s="369"/>
+      <c r="F1" s="369"/>
+      <c r="G1" s="369"/>
+      <c r="H1" s="370"/>
+      <c r="I1" s="368" t="s">
         <v>312</v>
       </c>
-      <c r="J1" s="372"/>
-      <c r="K1" s="372"/>
-      <c r="L1" s="372"/>
-      <c r="M1" s="373"/>
-      <c r="N1" s="368" t="s">
+      <c r="J1" s="369"/>
+      <c r="K1" s="369"/>
+      <c r="L1" s="369"/>
+      <c r="M1" s="370"/>
+      <c r="N1" s="371" t="s">
         <v>307</v>
       </c>
-      <c r="O1" s="369"/>
-      <c r="P1" s="369"/>
-      <c r="Q1" s="369"/>
-      <c r="R1" s="370"/>
-      <c r="S1" s="368" t="s">
+      <c r="O1" s="372"/>
+      <c r="P1" s="372"/>
+      <c r="Q1" s="372"/>
+      <c r="R1" s="373"/>
+      <c r="S1" s="371" t="s">
         <v>308</v>
       </c>
-      <c r="T1" s="369"/>
-      <c r="U1" s="369"/>
-      <c r="V1" s="369"/>
-      <c r="W1" s="370"/>
-      <c r="X1" s="368" t="s">
+      <c r="T1" s="372"/>
+      <c r="U1" s="372"/>
+      <c r="V1" s="372"/>
+      <c r="W1" s="373"/>
+      <c r="X1" s="371" t="s">
         <v>309</v>
       </c>
-      <c r="Y1" s="369"/>
-      <c r="Z1" s="369"/>
-      <c r="AA1" s="369"/>
-      <c r="AB1" s="370"/>
-      <c r="AC1" s="368" t="s">
+      <c r="Y1" s="372"/>
+      <c r="Z1" s="372"/>
+      <c r="AA1" s="372"/>
+      <c r="AB1" s="373"/>
+      <c r="AC1" s="371" t="s">
         <v>310</v>
       </c>
-      <c r="AD1" s="369"/>
-      <c r="AE1" s="369"/>
-      <c r="AF1" s="369"/>
-      <c r="AG1" s="370"/>
-      <c r="AH1" s="368" t="s">
+      <c r="AD1" s="372"/>
+      <c r="AE1" s="372"/>
+      <c r="AF1" s="372"/>
+      <c r="AG1" s="373"/>
+      <c r="AH1" s="371" t="s">
         <v>313</v>
       </c>
-      <c r="AI1" s="369"/>
-      <c r="AJ1" s="369"/>
-      <c r="AK1" s="369"/>
-      <c r="AL1" s="370"/>
-      <c r="AM1" s="368" t="s">
+      <c r="AI1" s="372"/>
+      <c r="AJ1" s="372"/>
+      <c r="AK1" s="372"/>
+      <c r="AL1" s="373"/>
+      <c r="AM1" s="371" t="s">
         <v>314</v>
       </c>
-      <c r="AN1" s="369"/>
-      <c r="AO1" s="369"/>
-      <c r="AP1" s="369"/>
-      <c r="AQ1" s="370"/>
-      <c r="AR1" s="368" t="s">
+      <c r="AN1" s="372"/>
+      <c r="AO1" s="372"/>
+      <c r="AP1" s="372"/>
+      <c r="AQ1" s="373"/>
+      <c r="AR1" s="371" t="s">
         <v>315</v>
       </c>
-      <c r="AS1" s="369"/>
-      <c r="AT1" s="369"/>
-      <c r="AU1" s="369"/>
-      <c r="AV1" s="370"/>
-      <c r="AW1" s="368" t="s">
+      <c r="AS1" s="372"/>
+      <c r="AT1" s="372"/>
+      <c r="AU1" s="372"/>
+      <c r="AV1" s="373"/>
+      <c r="AW1" s="371" t="s">
         <v>316</v>
       </c>
-      <c r="AX1" s="369"/>
-      <c r="AY1" s="369"/>
-      <c r="AZ1" s="369"/>
-      <c r="BA1" s="370"/>
+      <c r="AX1" s="372"/>
+      <c r="AY1" s="372"/>
+      <c r="AZ1" s="372"/>
+      <c r="BA1" s="373"/>
       <c r="BE1" s="217"/>
     </row>
     <row r="2" spans="1:62" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -38750,16 +38717,16 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="nLBYnfUIXBD4z902H4QrQuY+e0Nz9JCcXHp2zsCNsdo8V8GZv/dlRyFH7HA1+fIwPLv98AbAxrSavDOrH8RRoQ==" saltValue="6kSdGsMLkeSILd6EoxhKuw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="10">
+    <mergeCell ref="AH1:AL1"/>
+    <mergeCell ref="AM1:AQ1"/>
+    <mergeCell ref="AR1:AV1"/>
+    <mergeCell ref="AW1:BA1"/>
+    <mergeCell ref="AC1:AG1"/>
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="N1:R1"/>
     <mergeCell ref="S1:W1"/>
     <mergeCell ref="X1:AB1"/>
-    <mergeCell ref="AH1:AL1"/>
-    <mergeCell ref="AM1:AQ1"/>
-    <mergeCell ref="AR1:AV1"/>
-    <mergeCell ref="AW1:BA1"/>
-    <mergeCell ref="AC1:AG1"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -38774,8 +38741,8 @@
   </sheetPr>
   <dimension ref="A1:AH132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38930,7 +38897,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="161">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="162" t="s">
         <v>351</v>
@@ -38986,7 +38953,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="162" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="E7" s="163" t="s">
         <v>176</v>
@@ -39036,7 +39003,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="161">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="162" t="s">
         <v>293</v>
@@ -39092,7 +39059,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="162" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="E9" s="163" t="s">
         <v>176</v>
@@ -39145,7 +39112,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="162" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="E10" s="163" t="s">
         <v>176</v>
@@ -39198,7 +39165,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="162" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="E11" s="163" t="s">
         <v>176</v>
@@ -39248,7 +39215,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="161">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="162" t="s">
         <v>347</v>
@@ -39301,7 +39268,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="161">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="162" t="s">
         <v>348</v>
@@ -39460,9 +39427,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="163"/>
-      <c r="D16" s="162" t="s">
-        <v>352</v>
-      </c>
+      <c r="D16" s="162"/>
       <c r="E16" s="163"/>
       <c r="F16" s="162"/>
       <c r="G16" s="163"/>
@@ -39483,9 +39448,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="163"/>
-      <c r="D17" s="162" t="s">
-        <v>362</v>
-      </c>
+      <c r="D17" s="162"/>
       <c r="E17" s="163"/>
       <c r="F17" s="162"/>
       <c r="G17" s="163"/>
@@ -39506,9 +39469,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="163"/>
-      <c r="D18" s="162" t="s">
-        <v>353</v>
-      </c>
+      <c r="D18" s="162"/>
       <c r="E18" s="163"/>
       <c r="F18" s="163"/>
       <c r="G18" s="163"/>
@@ -39529,9 +39490,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="163"/>
-      <c r="D19" s="162" t="s">
-        <v>354</v>
-      </c>
+      <c r="D19" s="162"/>
       <c r="E19" s="164"/>
       <c r="F19" s="164"/>
       <c r="G19" s="164"/>
@@ -39552,9 +39511,7 @@
         <v>15</v>
       </c>
       <c r="C20" s="163"/>
-      <c r="D20" s="162" t="s">
-        <v>355</v>
-      </c>
+      <c r="D20" s="162"/>
       <c r="E20" s="163"/>
       <c r="F20" s="162"/>
       <c r="G20" s="163"/>
@@ -39575,9 +39532,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="163"/>
-      <c r="D21" s="162" t="s">
-        <v>356</v>
-      </c>
+      <c r="D21" s="162"/>
       <c r="E21" s="163"/>
       <c r="F21" s="162"/>
       <c r="G21" s="163"/>
@@ -39598,9 +39553,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="163"/>
-      <c r="D22" s="162" t="s">
-        <v>357</v>
-      </c>
+      <c r="D22" s="162"/>
       <c r="E22" s="163"/>
       <c r="F22" s="162"/>
       <c r="G22" s="163"/>
@@ -39621,9 +39574,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="163"/>
-      <c r="D23" s="162" t="s">
-        <v>361</v>
-      </c>
+      <c r="D23" s="162"/>
       <c r="E23" s="163"/>
       <c r="F23" s="162"/>
       <c r="G23" s="163"/>
@@ -39644,9 +39595,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="163"/>
-      <c r="D24" s="162" t="s">
-        <v>358</v>
-      </c>
+      <c r="D24" s="162"/>
       <c r="E24" s="163"/>
       <c r="F24" s="162"/>
       <c r="G24" s="163"/>
@@ -39667,9 +39616,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="163"/>
-      <c r="D25" s="162" t="s">
-        <v>359</v>
-      </c>
+      <c r="D25" s="162"/>
       <c r="E25" s="163"/>
       <c r="F25" s="162"/>
       <c r="G25" s="163"/>
@@ -39690,9 +39637,7 @@
         <v>21</v>
       </c>
       <c r="C26" s="163"/>
-      <c r="D26" s="162" t="s">
-        <v>360</v>
-      </c>
+      <c r="D26" s="162"/>
       <c r="E26" s="163"/>
       <c r="F26" s="162"/>
       <c r="G26" s="163"/>
@@ -43013,7 +42958,7 @@
       </c>
       <c r="B10" s="140">
         <f>IF(PROJ!C13="","",IF(B9="","",PROJ!C13))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="141">
@@ -45669,7 +45614,7 @@
       </c>
       <c r="B10" s="140">
         <f>IF(PROJ!C13="","",IF(B9="","",PROJ!C13))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="141">
@@ -48080,7 +48025,7 @@
       </c>
       <c r="B10" s="140">
         <f>IF(PROJ!C13="","",IF(B9="","",PROJ!C13))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="151"/>
@@ -51277,7 +51222,7 @@
       </c>
       <c r="B10" s="140">
         <f>IF(PROJ!C13="","",IF(B9="","",PROJ!C13))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="26"/>

</xml_diff>